<commit_message>
Added the regexs for the FORMATION block, need to implement them in the code
</commit_message>
<xml_diff>
--- a/venv/cv.xlsx
+++ b/venv/cv.xlsx
@@ -14,81 +14,360 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
-  <si>
-    <t>Myrvete HATOUM</t>
-  </si>
-  <si>
-    <t>Apprentie ingénieure en Systèmes d'Information chez InfoPro Digital</t>
-  </si>
-  <si>
-    <t>myrvete.hatoum@gmail.com</t>
-  </si>
-  <si>
-    <t>Summary</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>Experience</t>
-  </si>
-  <si>
-    <t>Développeuse web at Infopro digital</t>
-  </si>
-  <si>
-    <t>septembre 2015  -  Present</t>
-  </si>
-  <si>
-    <t>Développeuse Java at Infopro digital</t>
-  </si>
-  <si>
-    <t>avril 2015  -  juin 2015 (3 mois)</t>
-  </si>
-  <si>
-    <t>Education</t>
-  </si>
-  <si>
-    <t>ECE Paris</t>
-  </si>
-  <si>
-    <t>Diplôme d'ingénieur en Systèmes d'Information, 2015 - 2018</t>
-  </si>
-  <si>
-    <t>Dublin Business School</t>
-  </si>
-  <si>
-    <t>Séminaire de business de trois semaines en partenariat avec l'ECE Paris, 2017 - 2017</t>
-  </si>
-  <si>
-    <t>Universidad Europea</t>
-  </si>
-  <si>
-    <t>Programme universitaire de trois mois en partenariat avec l'ECE Paris, 2016 - 2016</t>
-  </si>
-  <si>
-    <t>Université Paris 13</t>
-  </si>
-  <si>
-    <t>DUT Informatique, 2013 - 2015</t>
-  </si>
-  <si>
-    <t>Université Paris Diderot</t>
-  </si>
-  <si>
-    <t>PACES , 2012 - 2013</t>
-  </si>
-  <si>
-    <t>Page 1</t>
-  </si>
-  <si>
-    <t>_x000C_Myrvete HATOUM</t>
-  </si>
-  <si>
-    <t>Contact Myrvete on LinkedIn</t>
-  </si>
-  <si>
-    <t>Page 2</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="119">
+  <si>
+    <t>Matteo Sammarco</t>
+  </si>
+  <si>
+    <t>Data Scientist</t>
+  </si>
+  <si>
+    <t>Issy-les-Moulineaux (92) - Email me on Indeed: indeed.com/r/Matteo-Sammarco/93bdbb4682ad23a5</t>
+  </si>
+  <si>
+    <t>EXPÉRIENCE</t>
+  </si>
+  <si>
+    <t>Axa Data Innovation Lab  -  Suresnes (92) -</t>
+  </si>
+  <si>
+    <t>octobre 2015 - actuellement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Data Science (Machine Learning, Deep Learning), </t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Insurance products, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Connected Car, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">- IoT, </t>
+  </si>
+  <si>
+    <t>- Mobile App (iOS and Android).</t>
+  </si>
+  <si>
+    <t>INGENIEUR R&amp;D</t>
+  </si>
+  <si>
+    <t>Université Pierre et Marie Curie  -  Paris (75) -</t>
+  </si>
+  <si>
+    <t>mai 2011 - actuellement</t>
+  </si>
+  <si>
+    <t>Paris, France.</t>
+  </si>
+  <si>
+    <t>{ Analyse statistique et corrélation de données. Analyse de traces Wi-Fi pour la dé- tection de comportements</t>
+  </si>
+  <si>
+    <t>malveillants, les activités des utilisateurs et la mesure des</t>
+  </si>
+  <si>
+    <t>performances du réseau.</t>
+  </si>
+  <si>
+    <t>{ Collecte et analyse des messages sur les réseaux sociaux (Twitter, Facebook et Sina</t>
+  </si>
+  <si>
+    <t>Weibo) et corrélation avec les niveaux de pollution de l'air dans le monde. Classification des messages avec</t>
+  </si>
+  <si>
+    <t>apprentissage automatique. Visualisation sur cartes géographiques.</t>
+  </si>
+  <si>
+    <t>{ Modélisation, analyse et visualisation de traces de mobilité.</t>
+  </si>
+  <si>
+    <t>{ Outils utilisés: R, Python avec Pandas, NetworkX et Matplotlib, scripting Bash, Awk,</t>
+  </si>
+  <si>
+    <t>Sed, Gnuplot, MongoDB, QGIS, Drake, Hadoop, Machine Learning.</t>
+  </si>
+  <si>
+    <t>Android et plateformes mobiles</t>
+  </si>
+  <si>
+    <t>{ Implémentation d'applications Android pour réseaux ad-hoc (dont transferts de fichiers</t>
+  </si>
+  <si>
+    <t>volumineux).</t>
+  </si>
+  <si>
+    <t>- Implémentation de protocoles réseaux distribués.</t>
+  </si>
+  <si>
+    <t>- Exploitation des communications IPv4, IPv6, Unicast, Broadcast, Multicast, Wi-Fi</t>
+  </si>
+  <si>
+    <t>Direct, Bluetooth 3.0 sur Android (SDK, NDK).</t>
+  </si>
+  <si>
+    <t>-  Implémentation  de:  (i)  PePiT  (mobile  data  offloading  app,  démo  presentée  dans  une  conférence</t>
+  </si>
+  <si>
+    <t>internationale), (ii) NTP Simple (synchronisation de l'horloge Android avec un serveur NTP), (iii) Cron Simple</t>
+  </si>
+  <si>
+    <t>(ordonnanceur de tâches), (iv) apps</t>
+  </si>
+  <si>
+    <t>personnelles publiées sur le Google Play Store et le Windows Phone Store</t>
+  </si>
+  <si>
+    <t>{ Responsable du développement et de la collaboration avec différents partenaires.</t>
+  </si>
+  <si>
+    <t>Réseaux et sécurité</t>
+  </si>
+  <si>
+    <t>{ Capture, traitement et analyse de traces Wi-Fi pour la détection de comportements</t>
+  </si>
+  <si>
+    <t>malveillants et la mesure des performances réseaux.</t>
+  </si>
+  <si>
+    <t>_x000C_{ Passage à l'échelle des systèmes de surveillance de réseau local sans fil avec deux</t>
+  </si>
+  <si>
+    <t>approches originales: (i) Sélection de traces basée sur leur similarité et sur des algorithmes de détection de</t>
+  </si>
+  <si>
+    <t>communautés de graphes, (ii) Mesures collaboratives avec</t>
+  </si>
+  <si>
+    <t>détection de comportements malveillants.</t>
+  </si>
+  <si>
+    <t>Véhicules connectés, systèmes de transport intelligents et réseaux véhiculaires</t>
+  </si>
+  <si>
+    <t>{ Développement d'une application Android pour la détection de places libres de parking avec Open Computer</t>
+  </si>
+  <si>
+    <t>Vision.</t>
+  </si>
+  <si>
+    <t>{ Integration de données de la pollution de l'air dans les systèmes de transport intelligents.</t>
+  </si>
+  <si>
+    <t>INGENIEUR R&amp;D, LINCS</t>
+  </si>
+  <si>
+    <t>Laboratory of Information, Networking and Communication Sciences  -  Paris (75) -</t>
+  </si>
+  <si>
+    <t>octobre 2010 - août 2014</t>
+  </si>
+  <si>
+    <t>France. Le LINCS (Laboratory of Information, Networking and Communication Sciences) est un laboratoire</t>
+  </si>
+  <si>
+    <t>commun d'informatique entre l'Inria, Alcatel-Lucent, SystemX, l'UPMC et</t>
+  </si>
+  <si>
+    <t>l'Institut Télécom (http://www.lincs.fr/about-us/).</t>
+  </si>
+  <si>
+    <t>{ Implémentation d'un système multi-agents en Java basé sur le modèle de mobilité SIMPS</t>
+  </si>
+  <si>
+    <t>("SIMPS: using sociology for personal mobility", V. Borrel, F. Legendre, M. Dias de</t>
+  </si>
+  <si>
+    <t>Amorim, S. Fdida, in IEEE/ACM Transactions on Networking).</t>
+  </si>
+  <si>
+    <t>CONSULTANT FREELANCE</t>
+  </si>
+  <si>
+    <t>GTI Voyages  -  Paris (75) -</t>
+  </si>
+  <si>
+    <t>août 2013 - août 2013</t>
+  </si>
+  <si>
+    <t>Algorithmes  de  pricing  dans  le  secteur  secteur  de  l'hôtellerie.  Diagnostic  et  mise  à  jour  des  systèmes</t>
+  </si>
+  <si>
+    <t>d'information de l'entreprise.</t>
+  </si>
+  <si>
+    <t>Télécom ParisTech  -  Paris (75) -</t>
+  </si>
+  <si>
+    <t>avril 2010 - avril 2011</t>
+  </si>
+  <si>
+    <t>Paris, France. Mise en place, gestion et réalisation d'expériences d'émulation réseau afin d'étudier</t>
+  </si>
+  <si>
+    <t>l'interaction entre les niveaux 7 et 3 de la pile OSI avec applications P2P-TV; analyse des résultats; gestion</t>
+  </si>
+  <si>
+    <t>d'une grille de sept serveurs Linux.</t>
+  </si>
+  <si>
+    <t>{ FP7 Moto http://www.fp7-moto.eu/</t>
+  </si>
+  <si>
+    <t>Partenaires: Centro Ricerche FIAT, Thales, Innovalia, CNR, Intecs, Fon, UPMC.</t>
+  </si>
+  <si>
+    <t>{ ANR Crowd http://anr-crowd.lip6.fr/</t>
+  </si>
+  <si>
+    <t>Partenaires: Thales, UPMC, 20Minutes.</t>
+  </si>
+  <si>
+    <t>{ ANR Rescue http://rescue.lille.inria.fr/</t>
+  </si>
+  <si>
+    <t>Partenaires: Inria, UPMC, Laboratoire d'Analyse et d'Architecture des Systèmes, France Telecom,</t>
+  </si>
+  <si>
+    <t>École Normale Supérieure de Lyon.</t>
+  </si>
+  <si>
+    <t>_x000C_{ FP7 NapaWine http://www.napa-wine.eu/cgi-bin/twiki/view/Public</t>
+  </si>
+  <si>
+    <t>Partenaires: France Telecom, Politecnico di Torino, Università di Trento, Budapest University of</t>
+  </si>
+  <si>
+    <t>Technology and Economics, Télécom ParisTech, LightComm, Magyar Telekom, Nec, NETvisor,</t>
+  </si>
+  <si>
+    <t>Telekomunikacja Polska, Warsaw University of Technology.</t>
+  </si>
+  <si>
+    <t>FORMATION</t>
+  </si>
+  <si>
+    <t>Doctorat en en Informatique</t>
+  </si>
+  <si>
+    <t>UPMC Sorbonne  -  Paris (75)</t>
+  </si>
+  <si>
+    <t>2014</t>
+  </si>
+  <si>
+    <t>Master en Informatique</t>
+  </si>
+  <si>
+    <t>Università degli Studi di Napoli Federico II  -  Napoli, Campania</t>
+  </si>
+  <si>
+    <t>2010</t>
+  </si>
+  <si>
+    <t>LIENS</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/public-profile/settings?trk=d_flagship3_profile_self_view_public_profile</t>
+  </si>
+  <si>
+    <t>INFORMATIONS COMPLÉMENTAIRES</t>
+  </si>
+  <si>
+    <t>Compétences informatiques</t>
+  </si>
+  <si>
+    <t>Développement Java, Bash, Sed, Awk, Python, C++, XML. Petits projets avec Perl, C#, VHDL,</t>
+  </si>
+  <si>
+    <t>Prolog, JavaScript, Assembly (Motorola 68000)</t>
+  </si>
+  <si>
+    <t>Data Science R, Python avec Pandas NetworkX et Matplotlib, Drake, scripting, machine learning,</t>
+  </si>
+  <si>
+    <t>Hadoop</t>
+  </si>
+  <si>
+    <t>Théorie des Algorithmes sur les graphes, Python NetworkX</t>
+  </si>
+  <si>
+    <t>graphes</t>
+  </si>
+  <si>
+    <t>OS Linux (Debian-like), Android, Microsoft Windows, Microsoft Windows Phone</t>
+  </si>
+  <si>
+    <t>BD MySQL, SQlite, MongoDB</t>
+  </si>
+  <si>
+    <t>Réseaux TCP/IP, Pile ISO OSI, IEEE 802.11, DTN, NDN, ICN, V2X</t>
+  </si>
+  <si>
+    <t>Logiciels RStudio, KNIME (apprentissage automatique et data mining), Wireshark, Wipal,</t>
+  </si>
+  <si>
+    <t>Wscout (Wi-Fi sniffer, trace analyzer), ModelNet-TE (émulation réseaux), Eclipse,</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Emacs, LTEX, R (calcul scientifique ), {Microsoft, Open, Libre}Office, Gnuplot,</t>
+  </si>
+  <si>
+    <t>SVN, GIT, GraphViz, VirtualBox, Visual Studio</t>
+  </si>
+  <si>
+    <t>Applications publiées</t>
+  </si>
+  <si>
+    <t>Google Play Code Civil et Pénal, Si Gonfia La Rete, Emacs Quick Reference, Code de la Route,</t>
+  </si>
+  <si>
+    <t>Code de la consommation</t>
+  </si>
+  <si>
+    <t>Windows Si Gonfia La Rete</t>
+  </si>
+  <si>
+    <t>Phone Store</t>
+  </si>
+  <si>
+    <t>Simulateur SIMPS, simulateur de mobilité des piétons</t>
+  </si>
+  <si>
+    <t>Systèmes d'information 30/30</t>
+  </si>
+  <si>
+    <t>Réseaux informatiques II 30/30</t>
+  </si>
+  <si>
+    <t>Génie logiciel II 30/30</t>
+  </si>
+  <si>
+    <t>_x000C_Algorithmes 30/30</t>
+  </si>
+  <si>
+    <t>2008 Licence en Ingénierie Informatique, Università degli Studi di Napoli Federico II,</t>
+  </si>
+  <si>
+    <t>Naples, Italie.</t>
+  </si>
+  <si>
+    <t>Mémoire: "A system to filter image-based spam emails".</t>
+  </si>
+  <si>
+    <t>2008 Cisco Certification CCNA1.</t>
+  </si>
+  <si>
+    <t>Evaluation: […]</t>
+  </si>
+  <si>
+    <t>2004 Diplôme baccalauréat scientifique, Naples, Italie.</t>
+  </si>
+  <si>
+    <t>Mention très bien […]</t>
   </si>
   <si>
     <t>_x000C_</t>
@@ -98,13 +377,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -124,13 +410,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -423,7 +715,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A38"/>
+  <dimension ref="A1:A166"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -434,142 +726,620 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" t="s">
-        <v>20</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>21</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>2</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>23</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
         <v>25</v>
       </c>
     </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1">
+      <c r="A124" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1">
+      <c r="A128" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1">
+      <c r="A130" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1">
+      <c r="A136" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1">
+      <c r="A137" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1">
+      <c r="A138" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1">
+      <c r="A139" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1">
+      <c r="A140" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1">
+      <c r="A141" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1">
+      <c r="A142" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1">
+      <c r="A143" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1">
+      <c r="A144" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1">
+      <c r="A145" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1">
+      <c r="A146" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1">
+      <c r="A147" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1">
+      <c r="A148" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1">
+      <c r="A149" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1">
+      <c r="A150" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1">
+      <c r="A152" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1">
+      <c r="A153" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1">
+      <c r="A154" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1">
+      <c r="A156" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1">
+      <c r="A158" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1">
+      <c r="A159" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1">
+      <c r="A160" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1">
+      <c r="A161" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1">
+      <c r="A162" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1">
+      <c r="A163" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1">
+      <c r="A164" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1">
+      <c r="A166" t="s">
+        <v>118</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A126" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>